<commit_message>
Running all scripts to evaluate the resučt
</commit_message>
<xml_diff>
--- a/dataSet/cleanData/cleanData.xlsx
+++ b/dataSet/cleanData/cleanData.xlsx
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:G310"/>
+  <dimension ref="A1:G311"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -8196,6 +8196,31 @@
         <v>32</v>
       </c>
     </row>
+    <row r="311">
+      <c r="A311" t="inlineStr">
+        <is>
+          <t>08.01.2021</t>
+        </is>
+      </c>
+      <c r="B311" t="n">
+        <v>114920</v>
+      </c>
+      <c r="C311" t="n">
+        <v>1528</v>
+      </c>
+      <c r="D311" t="n">
+        <v>3280815</v>
+      </c>
+      <c r="E311" t="n">
+        <v>513</v>
+      </c>
+      <c r="F311" t="n">
+        <v>2623</v>
+      </c>
+      <c r="G311" t="n">
+        <v>32</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>